<commit_message>
save the PAM data!
</commit_message>
<xml_diff>
--- a/metadata/rlc_metadata_06172024.xlsx
+++ b/metadata/rlc_metadata_06172024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssdon\OneDrive\Documents\github\anemone-leachate-heat\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D2514C-49FB-438E-A21E-ECCD47853777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1747A4DA-6FE9-4089-94CF-0E6233BA796A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="75">
   <si>
     <t>sample_id</t>
   </si>
@@ -235,6 +235,21 @@
   </si>
   <si>
     <t>A7C</t>
+  </si>
+  <si>
+    <t>ambient</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>A. elegantissima x B. muscatinei</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>low</t>
   </si>
 </sst>
 </file>
@@ -553,11 +568,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -565,7 +580,7 @@
     <col min="3" max="3" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -587,8 +602,11 @@
       <c r="G1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -607,8 +625,11 @@
       <c r="F2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>14</v>
       </c>
@@ -618,8 +639,20 @@
       <c r="C3" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>27</v>
       </c>
@@ -629,8 +662,20 @@
       <c r="C4" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>53</v>
       </c>
@@ -640,8 +685,20 @@
       <c r="C5" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>73</v>
       </c>
@@ -651,8 +708,20 @@
       <c r="C6" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>86</v>
       </c>
@@ -662,8 +731,20 @@
       <c r="C7" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>99</v>
       </c>
@@ -673,8 +754,20 @@
       <c r="C8" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>112</v>
       </c>
@@ -684,8 +777,20 @@
       <c r="C9" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>125</v>
       </c>
@@ -695,8 +800,20 @@
       <c r="C10" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>138</v>
       </c>
@@ -706,8 +823,20 @@
       <c r="C11" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>151</v>
       </c>
@@ -717,8 +846,20 @@
       <c r="C12" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>164</v>
       </c>
@@ -728,8 +869,20 @@
       <c r="C13" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>177</v>
       </c>
@@ -739,8 +892,20 @@
       <c r="C14" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>190</v>
       </c>
@@ -750,8 +915,20 @@
       <c r="C15" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>203</v>
       </c>
@@ -761,8 +938,20 @@
       <c r="C16" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>216</v>
       </c>
@@ -772,8 +961,20 @@
       <c r="C17" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>229</v>
       </c>
@@ -783,8 +984,20 @@
       <c r="C18" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>242</v>
       </c>
@@ -794,8 +1007,20 @@
       <c r="C19" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>255</v>
       </c>
@@ -805,8 +1030,20 @@
       <c r="C20" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>268</v>
       </c>
@@ -816,8 +1053,20 @@
       <c r="C21" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>281</v>
       </c>
@@ -827,8 +1076,20 @@
       <c r="C22" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>294</v>
       </c>
@@ -838,8 +1099,20 @@
       <c r="C23" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>307</v>
       </c>
@@ -849,8 +1122,20 @@
       <c r="C24" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>320</v>
       </c>
@@ -860,8 +1145,20 @@
       <c r="C25" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>346</v>
       </c>
@@ -871,8 +1168,20 @@
       <c r="C26" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>359</v>
       </c>
@@ -882,8 +1191,20 @@
       <c r="C27" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>372</v>
       </c>
@@ -893,8 +1214,20 @@
       <c r="C28" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>385</v>
       </c>
@@ -904,8 +1237,20 @@
       <c r="C29" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>398</v>
       </c>
@@ -915,8 +1260,20 @@
       <c r="C30" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>411</v>
       </c>
@@ -926,8 +1283,20 @@
       <c r="C31" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>424</v>
       </c>
@@ -937,8 +1306,20 @@
       <c r="C32" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>437</v>
       </c>
@@ -948,8 +1329,20 @@
       <c r="C33" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D33" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>450</v>
       </c>
@@ -959,11 +1352,23 @@
       <c r="C34" s="1">
         <v>45460</v>
       </c>
+      <c r="D34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s">
+        <v>74</v>
+      </c>
       <c r="G34" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>463</v>
       </c>
@@ -973,11 +1378,23 @@
       <c r="C35" s="1">
         <v>45460</v>
       </c>
+      <c r="D35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35" t="s">
+        <v>74</v>
+      </c>
       <c r="G35" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>476</v>
       </c>
@@ -987,8 +1404,20 @@
       <c r="C36" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>73</v>
+      </c>
+      <c r="H36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>489</v>
       </c>
@@ -998,8 +1427,20 @@
       <c r="C37" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D37" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
+      <c r="H37" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>502</v>
       </c>
@@ -1009,8 +1450,20 @@
       <c r="C38" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E38">
+        <v>8</v>
+      </c>
+      <c r="F38" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>515</v>
       </c>
@@ -1020,8 +1473,20 @@
       <c r="C39" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
+      <c r="F39" t="s">
+        <v>74</v>
+      </c>
+      <c r="H39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>528</v>
       </c>
@@ -1031,8 +1496,20 @@
       <c r="C40" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="F40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>541</v>
       </c>
@@ -1042,8 +1519,20 @@
       <c r="C41" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D41" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
+        <v>74</v>
+      </c>
+      <c r="H41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>555</v>
       </c>
@@ -1053,8 +1542,20 @@
       <c r="C42" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>568</v>
       </c>
@@ -1064,8 +1565,20 @@
       <c r="C43" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>73</v>
+      </c>
+      <c r="H43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>581</v>
       </c>
@@ -1075,8 +1588,20 @@
       <c r="C44" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D44" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>594</v>
       </c>
@@ -1086,8 +1611,20 @@
       <c r="C45" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45">
+        <v>6</v>
+      </c>
+      <c r="F45" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>607</v>
       </c>
@@ -1097,8 +1634,20 @@
       <c r="C46" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
+        <v>74</v>
+      </c>
+      <c r="H46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>620</v>
       </c>
@@ -1108,8 +1657,20 @@
       <c r="C47" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D47" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47">
+        <v>7</v>
+      </c>
+      <c r="F47" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>633</v>
       </c>
@@ -1119,8 +1680,20 @@
       <c r="C48" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D48" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48">
+        <v>9</v>
+      </c>
+      <c r="F48" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>646</v>
       </c>
@@ -1130,8 +1703,20 @@
       <c r="C49" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D49" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>73</v>
+      </c>
+      <c r="H49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>659</v>
       </c>
@@ -1141,8 +1726,20 @@
       <c r="C50" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D50" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s">
+        <v>32</v>
+      </c>
+      <c r="H50" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>672</v>
       </c>
@@ -1152,8 +1749,20 @@
       <c r="C51" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D51" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="F51" t="s">
+        <v>73</v>
+      </c>
+      <c r="H51" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>685</v>
       </c>
@@ -1163,8 +1772,20 @@
       <c r="C52" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D52" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
+        <v>74</v>
+      </c>
+      <c r="H52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>698</v>
       </c>
@@ -1174,8 +1795,20 @@
       <c r="C53" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D53" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53">
+        <v>10</v>
+      </c>
+      <c r="F53" t="s">
+        <v>73</v>
+      </c>
+      <c r="H53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>711</v>
       </c>
@@ -1185,8 +1818,20 @@
       <c r="C54" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D54" t="s">
+        <v>31</v>
+      </c>
+      <c r="E54">
+        <v>6</v>
+      </c>
+      <c r="F54" t="s">
+        <v>73</v>
+      </c>
+      <c r="H54" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>731</v>
       </c>
@@ -1196,8 +1841,20 @@
       <c r="C55" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D55" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>74</v>
+      </c>
+      <c r="H55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>744</v>
       </c>
@@ -1207,8 +1864,20 @@
       <c r="C56" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D56" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56">
+        <v>10</v>
+      </c>
+      <c r="F56" t="s">
+        <v>74</v>
+      </c>
+      <c r="H56" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>757</v>
       </c>
@@ -1218,8 +1887,20 @@
       <c r="C57" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57">
+        <v>6</v>
+      </c>
+      <c r="F57" t="s">
+        <v>74</v>
+      </c>
+      <c r="H57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>770</v>
       </c>
@@ -1229,8 +1910,20 @@
       <c r="C58" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D58" t="s">
+        <v>70</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
+        <v>32</v>
+      </c>
+      <c r="H58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>783</v>
       </c>
@@ -1240,8 +1933,20 @@
       <c r="C59" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D59" t="s">
+        <v>70</v>
+      </c>
+      <c r="E59">
+        <v>4</v>
+      </c>
+      <c r="F59" t="s">
+        <v>74</v>
+      </c>
+      <c r="H59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>796</v>
       </c>
@@ -1251,8 +1956,20 @@
       <c r="C60" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D60" t="s">
+        <v>70</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="F60" t="s">
+        <v>73</v>
+      </c>
+      <c r="H60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>809</v>
       </c>
@@ -1262,8 +1979,20 @@
       <c r="C61" s="1">
         <v>45460</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D61" t="s">
+        <v>31</v>
+      </c>
+      <c r="E61">
+        <v>7</v>
+      </c>
+      <c r="F61" t="s">
+        <v>73</v>
+      </c>
+      <c r="H61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>822</v>
       </c>
@@ -1272,6 +2001,18 @@
       </c>
       <c r="C62" s="1">
         <v>45460</v>
+      </c>
+      <c r="D62" t="s">
+        <v>70</v>
+      </c>
+      <c r="E62">
+        <v>7</v>
+      </c>
+      <c r="F62" t="s">
+        <v>73</v>
+      </c>
+      <c r="H62" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>